<commit_message>
new basic stats 2022
</commit_message>
<xml_diff>
--- a/plots/basic_stats/single_var_stats/allmus_summary_var-accreditation.xlsx
+++ b/plots/basic_stats/single_var_stats/allmus_summary_var-accreditation.xlsx
@@ -386,10 +386,10 @@
         </is>
       </c>
       <c r="B2">
-        <v>2326</v>
+        <v>2508</v>
       </c>
       <c r="C2">
-        <v>57.98</v>
+        <v>59.3</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -404,10 +404,10 @@
         </is>
       </c>
       <c r="B3">
-        <v>1686</v>
+        <v>1721</v>
       </c>
       <c r="C3">
-        <v>42.02</v>
+        <v>40.7</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>

</xml_diff>